<commit_message>
Actualización de archivos 2
</commit_message>
<xml_diff>
--- a/HospitalOk.xlsx
+++ b/HospitalOk.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>ENFERMEDAD CRONICA PULMONAR OBSTRUCTIVA</t>
+          <t>EPOC</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>COMPLICACION INFECCIOSA POST BIOPSIA</t>
+          <t>COMPLICACION POST BIOPSIA</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">

</xml_diff>